<commit_message>
filling in some blanks
</commit_message>
<xml_diff>
--- a/tax-exempt-status/501ctypes.xlsx
+++ b/tax-exempt-status/501ctypes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviabeck/Box Sync/metadata-standards/tax-exempt-status/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D732D0-81A8-094A-B785-AE24379165E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F79C48A-4AE8-674D-B130-049403A56A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{96359B12-0556-B241-B8CB-31DA73770B59}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{96359B12-0556-B241-B8CB-31DA73770B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="key" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="155">
   <si>
     <t>label</t>
   </si>
@@ -611,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,8 +653,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1075,13 +1074,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CEA9CEF-B507-344B-BD8D-D89C17498ABD}" name="Table2" displayName="Table2" ref="A1:D1048575" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CEA9CEF-B507-344B-BD8D-D89C17498ABD}" name="Table2" displayName="Table2" ref="A1:D1048575" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A1:D1048575" xr:uid="{5CEA9CEF-B507-344B-BD8D-D89C17498ABD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C3C13462-3393-4149-A4F5-9569FC4FF31C}" name="Variable " dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{E53B42F8-4674-EF4F-8EE2-56EAD3F36E70}" name="Value" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{B657E8B2-2909-154D-A601-D2AC4802F5AC}" name="Meaning" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{DA400F18-BC25-774E-B308-2D153F8855E0}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C3C13462-3393-4149-A4F5-9569FC4FF31C}" name="Variable " dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E53B42F8-4674-EF4F-8EE2-56EAD3F36E70}" name="Value" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B657E8B2-2909-154D-A601-D2AC4802F5AC}" name="Meaning" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{DA400F18-BC25-774E-B308-2D153F8855E0}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1386,9 +1385,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE3B902-8DA6-D346-AFF8-0B0CB0AD27B0}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="92" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2007,7 +2006,9 @@
       <c r="F17" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="11" t="s">
+        <v>123</v>
+      </c>
       <c r="H17" s="11" t="s">
         <v>3</v>
       </c>
@@ -2779,10 +2780,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="83.83203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="137.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="83.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="137.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2800,391 +2801,391 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" t="s">
         <v>114</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" t="s">
         <v>116</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="A18" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+      <c r="A19" t="s">
         <v>114</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" t="s">
         <v>121</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
+      <c r="A21" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
+      <c r="A22" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
+      <c r="A23" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" s="17" t="s">
+      <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" t="s">
         <v>127</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="A25" t="s">
         <v>127</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="17" t="s">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+      <c r="A26" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C26" s="17" t="s">
+      <c r="B26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
+      <c r="A27" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="17" t="s">
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
+      <c r="A28" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" t="s">
         <v>134</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" t="s">
         <v>154</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
+      <c r="A30" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C30" s="17" t="s">
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
+      <c r="A31" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="17" t="s">
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
+      <c r="A32" t="s">
         <v>138</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
+      <c r="A33" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+      <c r="A34" t="s">
         <v>147</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
+      <c r="A35" t="s">
         <v>147</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
+      <c r="A36" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="17" t="s">
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
revised category labels for tax exempt status types
</commit_message>
<xml_diff>
--- a/tax-exempt-status/501ctypes.xlsx
+++ b/tax-exempt-status/501ctypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdlec\Dropbox (Personal)\00 - URBAN\00-GITHUB\metadata-standards\tax-exempt-status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4661EFC9-6E6E-4DD6-830D-E09484CB31AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3E0F3-10FB-41E3-A9CE-1FA91C722C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="3600" windowWidth="25200" windowHeight="16980" activeTab="1" xr2:uid="{96359B12-0556-B241-B8CB-31DA73770B59}"/>
+    <workbookView xWindow="13560" yWindow="3600" windowWidth="33480" windowHeight="16980" activeTab="1" xr2:uid="{96359B12-0556-B241-B8CB-31DA73770B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,13 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="161">
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="187">
   <si>
     <t>Notes</t>
   </si>
@@ -402,9 +396,6 @@
     <t>memership_restrictions</t>
   </si>
   <si>
-    <t>membership_restrictions</t>
-  </si>
-  <si>
     <t xml:space="preserve">no membership restrictions </t>
   </si>
   <si>
@@ -468,9 +459,6 @@
     <t>other_filing_requirements</t>
   </si>
   <si>
-    <t>other_filing_requirments</t>
-  </si>
-  <si>
     <t>list of forms other than 990 that this org type is required to file</t>
   </si>
   <si>
@@ -516,10 +504,100 @@
     <t>LEVEL1</t>
   </si>
   <si>
-    <t>NO_Y; NO_N</t>
-  </si>
-  <si>
-    <t>donations_ded_exception</t>
+    <t>501c</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>SOCIETAL</t>
+  </si>
+  <si>
+    <t>MEMBERSHIP</t>
+  </si>
+  <si>
+    <t>COOPERATIVE</t>
+  </si>
+  <si>
+    <t>MEMBER</t>
+  </si>
+  <si>
+    <t>GENERAL</t>
+  </si>
+  <si>
+    <t>CORPORATION</t>
+  </si>
+  <si>
+    <t>INSURANCE</t>
+  </si>
+  <si>
+    <t>DEFUNCT</t>
+  </si>
+  <si>
+    <t>PENSION</t>
+  </si>
+  <si>
+    <t>SPECIAL INT GRP</t>
+  </si>
+  <si>
+    <t>RESTRICTED</t>
+  </si>
+  <si>
+    <t>UNLIMITED</t>
+  </si>
+  <si>
+    <t>REGULAR</t>
+  </si>
+  <si>
+    <t>LIMITED</t>
+  </si>
+  <si>
+    <t>LODGE</t>
+  </si>
+  <si>
+    <t>INDEPENDENT</t>
+  </si>
+  <si>
+    <t>PF_N (can't file 990EZ if a PF)</t>
+  </si>
+  <si>
+    <t>FEDERAL</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>NO REQ</t>
+  </si>
+  <si>
+    <t>NEW VALUE</t>
+  </si>
+  <si>
+    <t>required_990 (is this 990EZ?)</t>
+  </si>
+  <si>
+    <t>exempt_type</t>
+  </si>
+  <si>
+    <t>exempt_subtype</t>
+  </si>
+  <si>
+    <t>member_restrict</t>
+  </si>
+  <si>
+    <t>supporting</t>
+  </si>
+  <si>
+    <t>SUBORDINATE (is subordinate the right label? DEPENDENT? LINKED?)</t>
+  </si>
+  <si>
+    <t>req_990</t>
+  </si>
+  <si>
+    <t>govt</t>
+  </si>
+  <si>
+    <t>donations_deduct</t>
   </si>
 </sst>
 </file>
@@ -571,7 +649,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -599,6 +677,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -647,7 +731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -689,25 +773,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="19">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -719,6 +835,56 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -762,100 +928,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1112,34 +1184,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65D72ABC-4F4D-F943-85DB-A2423E37D167}" name="Table1" displayName="Table1" ref="A1:M38" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <tableColumns count="13">
-    <tableColumn id="3" xr3:uid="{A3515E12-7EA5-CA4D-A295-2EF03ACFEEFC}" name="label" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{D6FD90D9-4201-9846-ACB0-312DAB2A3898}" name="Description" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{C9FB6DDE-A4A1-A141-AA8B-AD9F10DFD751}" name="tax_exempt_group" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{DBC925D3-0E81-6647-856B-F069B914912E}" name="tax_exempt_subgroup" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{614E85D6-D3FE-4B49-B673-3B96B127C892}" name="donations_deductible" dataDxfId="13"/>
-    <tableColumn id="1" xr3:uid="{4B05E01F-8F4B-4966-8332-67EA2A603F5A}" name="donations_ded_exception" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{C82BB2F4-5690-7E45-9989-0E6197C10A88}" name="political_activity" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{77957644-0E53-0447-8131-F726B2193A55}" name="memership_restrictions" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{8EB2C594-11DD-F04E-8BB4-D5AD8A946BA7}" name="existance_501c" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{5DBFDAB8-07D2-2C49-98EE-6FE49071B588}" name="required_990" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{72730379-06F2-2C42-ACEF-A5A28D1093BE}" name="option_990EZ" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{AD5A5539-ADEA-B747-A32F-06989F8D15A7}" name="other_filing_requirements" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{1DE016B8-130D-0F4E-AC4A-966AFC0590EB}" name="govt_established" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65D72ABC-4F4D-F943-85DB-A2423E37D167}" name="Table1" displayName="Table1" ref="A1:L38" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <tableColumns count="12">
+    <tableColumn id="3" xr3:uid="{A3515E12-7EA5-CA4D-A295-2EF03ACFEEFC}" name="501c" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{D6FD90D9-4201-9846-ACB0-312DAB2A3898}" name="description" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{C9FB6DDE-A4A1-A141-AA8B-AD9F10DFD751}" name="tax_exempt_group" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{DBC925D3-0E81-6647-856B-F069B914912E}" name="tax_exempt_subgroup" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{1DE016B8-130D-0F4E-AC4A-966AFC0590EB}" name="govt_established" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{5DBFDAB8-07D2-2C49-98EE-6FE49071B588}" name="required_990" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{72730379-06F2-2C42-ACEF-A5A28D1093BE}" name="option_990EZ" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{614E85D6-D3FE-4B49-B673-3B96B127C892}" name="donations_deductible" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{C82BB2F4-5690-7E45-9989-0E6197C10A88}" name="political_activity" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{77957644-0E53-0447-8131-F726B2193A55}" name="memership_restrictions" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{8EB2C594-11DD-F04E-8BB4-D5AD8A946BA7}" name="existance_501c" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{AD5A5539-ADEA-B747-A32F-06989F8D15A7}" name="other_filing_requirements" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CEA9CEF-B507-344B-BD8D-D89C17498ABD}" name="Table2" displayName="Table2" ref="B1:E1048575" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="B1:E1048575" xr:uid="{5CEA9CEF-B507-344B-BD8D-D89C17498ABD}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C3C13462-3393-4149-A4F5-9569FC4FF31C}" name="Variable " dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{E53B42F8-4674-EF4F-8EE2-56EAD3F36E70}" name="Value" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{B657E8B2-2909-154D-A601-D2AC4802F5AC}" name="Meaning" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{DA400F18-BC25-774E-B308-2D153F8855E0}" name="Notes" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CEA9CEF-B507-344B-BD8D-D89C17498ABD}" name="Table2" displayName="Table2" ref="B1:F1048575" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="B1:F1048575" xr:uid="{5CEA9CEF-B507-344B-BD8D-D89C17498ABD}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C3C13462-3393-4149-A4F5-9569FC4FF31C}" name="Variable " dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E53B42F8-4674-EF4F-8EE2-56EAD3F36E70}" name="Value" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2E6B336E-2674-40BC-B890-99248060995D}" name="NEW VALUE"/>
+    <tableColumn id="3" xr3:uid="{B657E8B2-2909-154D-A601-D2AC4802F5AC}" name="Meaning" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{DA400F18-BC25-774E-B308-2D153F8855E0}" name="Notes" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1446,7 +1518,7 @@
   <sheetViews>
     <sheetView zoomScale="92" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F6" sqref="F6"/>
+      <selection pane="topRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1455,1413 +1527,1409 @@
     <col min="2" max="2" width="120.125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.625" style="4" customWidth="1"/>
     <col min="4" max="4" width="31.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="25" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="24.125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="26.125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="24.375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="35.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="10.875" style="4"/>
+    <col min="6" max="6" width="26.125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="24.375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="24.125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="35" customWidth="1"/>
+    <col min="14" max="14" width="35.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>70</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>147</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="10"/>
+        <v>144</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>1</v>
+      </c>
       <c r="G2" s="10" t="s">
-        <v>118</v>
+        <v>2</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>148</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>120</v>
+      </c>
       <c r="G3" s="11" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L3" s="11"/>
-      <c r="M3" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>154</v>
+        <v>116</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="L4" s="10"/>
-      <c r="M4" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>115</v>
+        <v>1</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>123</v>
+        <v>113</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="L5" s="10"/>
-      <c r="M5" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
-        <v>115</v>
+        <v>1</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>113</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L6" s="11"/>
-      <c r="M6" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
-        <v>115</v>
+        <v>1</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>123</v>
+        <v>113</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="L7" s="10"/>
-      <c r="M7" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="L8" s="10"/>
-      <c r="M8" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>129</v>
+        <v>106</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="L9" s="11"/>
-      <c r="M9" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="L10" s="10"/>
-      <c r="M10" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>129</v>
+        <v>106</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="L11" s="11"/>
-      <c r="M11" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="L12" s="10"/>
-      <c r="M12" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L13" s="11"/>
-      <c r="M13" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="L14" s="10"/>
-      <c r="M14" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10" t="s">
-        <v>118</v>
+        <v>145</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L15" s="11"/>
-      <c r="M15" s="11" t="s">
-        <v>149</v>
-      </c>
+      <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L16" s="11"/>
-      <c r="M16" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L17" s="11"/>
-      <c r="M17" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L18" s="11"/>
-      <c r="M18" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L19" s="11"/>
-      <c r="M19" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>3</v>
+        <v>103</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L20" s="11"/>
-      <c r="M20" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="G21" s="10" t="s">
-        <v>118</v>
+        <v>2</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L21" s="10"/>
-      <c r="M21" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="M21" s="4"/>
     </row>
     <row r="22" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>123</v>
+        <v>103</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L22" s="11"/>
-      <c r="M22" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M22" s="4"/>
     </row>
     <row r="23" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="G23" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="13"/>
-      <c r="J23" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>123</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="13"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="10" t="s">
-        <v>3</v>
-      </c>
+      <c r="M23" s="4"/>
     </row>
     <row r="24" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="G24" s="11" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>123</v>
+        <v>113</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L24" s="11"/>
-      <c r="M24" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D25" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>4</v>
+      <c r="I25" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L25" s="11"/>
-      <c r="M25" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="M25" s="4"/>
     </row>
     <row r="26" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>123</v>
+        <v>103</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L26" s="11"/>
-      <c r="M26" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="M26" s="4"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10" t="s">
-        <v>118</v>
+        <v>145</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27" s="14" t="s">
-        <v>123</v>
+        <v>103</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L27" s="11"/>
-      <c r="M27" s="11" t="s">
-        <v>149</v>
-      </c>
+      <c r="M27" s="4"/>
     </row>
     <row r="28" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10" t="s">
-        <v>118</v>
+        <v>145</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>123</v>
+        <v>103</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L28" s="11"/>
-      <c r="M28" s="11" t="s">
-        <v>149</v>
-      </c>
+      <c r="M28" s="4"/>
     </row>
     <row r="29" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>99</v>
-      </c>
       <c r="E29" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>123</v>
+        <v>103</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L29" s="12"/>
-      <c r="M29" s="12" t="s">
-        <v>3</v>
-      </c>
+      <c r="M29" s="4"/>
     </row>
     <row r="30" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="C30" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="10" t="s">
-        <v>118</v>
+        <v>1</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>123</v>
+        <v>103</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L30" s="12"/>
-      <c r="M30" s="12" t="s">
-        <v>3</v>
-      </c>
+      <c r="M30" s="4"/>
     </row>
     <row r="31" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="H31" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>3</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="I31" s="16"/>
       <c r="J31" s="6" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>3</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="M31" s="4"/>
     </row>
     <row r="32" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="H32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>123</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="I32" s="16"/>
       <c r="J32" s="6" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L32" s="6"/>
-      <c r="M32" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="M32" s="4"/>
     </row>
     <row r="33" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" s="6"/>
-      <c r="G33" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="H33" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>123</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="I33" s="16"/>
       <c r="J33" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L33" s="6"/>
-      <c r="M33" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="M33" s="4"/>
     </row>
     <row r="34" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F34" s="6"/>
-      <c r="G34" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="H34" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>3</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="I34" s="16"/>
       <c r="J34" s="6" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="L34" s="6"/>
-      <c r="M34" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="M34" s="4"/>
     </row>
     <row r="35" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="H35" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>123</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="I35" s="16"/>
       <c r="J35" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L35" s="6"/>
-      <c r="M35" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B36" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>85</v>
-      </c>
       <c r="E36" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="H36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>3</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="I36" s="16"/>
       <c r="J36" s="6" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L36" s="6"/>
-      <c r="M36" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="M36" s="4"/>
     </row>
     <row r="37" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="H37" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>3</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="I37" s="16"/>
       <c r="J37" s="6" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L37" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>3</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="M37" s="4"/>
     </row>
     <row r="38" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F38" s="6"/>
-      <c r="G38" s="16"/>
+        <v>145</v>
+      </c>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
       <c r="H38" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
+        <v>103</v>
+      </c>
+      <c r="I38" s="16"/>
+      <c r="J38" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="L38" s="15"/>
-      <c r="M38" s="6" t="s">
-        <v>149</v>
-      </c>
+      <c r="M38" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2874,473 +2942,560 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD4381-EA25-4248-8CB2-EADFAADE5A2B}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.25" customWidth="1"/>
-    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.625" customWidth="1"/>
-    <col min="4" max="4" width="83.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="137.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.75" style="22" customWidth="1"/>
+    <col min="3" max="4" width="24.625" customWidth="1"/>
+    <col min="5" max="5" width="83.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="137.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
         <v>76</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" s="17" t="s">
+      <c r="E15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" t="s">
         <v>126</v>
       </c>
-      <c r="C12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D14" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" t="s">
-        <v>116</v>
-      </c>
-      <c r="E17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B18" t="s">
-        <v>114</v>
-      </c>
-      <c r="C18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" t="s">
-        <v>114</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="D24" t="s">
+        <v>171</v>
+      </c>
+      <c r="E24" t="s">
         <v>127</v>
       </c>
-      <c r="C23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>172</v>
+      </c>
+      <c r="E25" t="s">
         <v>128</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>127</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
         <v>134</v>
       </c>
-      <c r="C26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="22" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B27" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B28" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B29" t="s">
-        <v>134</v>
-      </c>
-      <c r="C29" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
         <v>138</v>
       </c>
-      <c r="C30" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="22" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E33" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>138</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
+        <v>174</v>
+      </c>
+      <c r="E34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C35" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>176</v>
+      </c>
+      <c r="E36" t="s">
         <v>147</v>
-      </c>
-      <c r="C34" t="s">
-        <v>148</v>
-      </c>
-      <c r="D34" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B35" t="s">
-        <v>147</v>
-      </c>
-      <c r="C35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B36" t="s">
-        <v>147</v>
-      </c>
-      <c r="C36" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating language for donations deductible. Fixing 501c19 information. Adding details to notes column.
</commit_message>
<xml_diff>
--- a/tax-exempt-status/501ctypes.xlsx
+++ b/tax-exempt-status/501ctypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviabeck/Box Sync/metadata-standards/tax-exempt-status/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2587C57-E9FC-F843-B00B-9CDA48360BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870AF53C-D0E9-5341-845E-7D195EF611B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{96359B12-0556-B241-B8CB-31DA73770B59}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{96359B12-0556-B241-B8CB-31DA73770B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="209">
   <si>
     <t>Notes</t>
   </si>
@@ -348,15 +348,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t xml:space="preserve">org can receive contribution - unrestricted </t>
-  </si>
-  <si>
-    <t xml:space="preserve">org can receive contribution under certain restrictions </t>
-  </si>
-  <si>
-    <t>YR</t>
-  </si>
-  <si>
     <t>YU</t>
   </si>
   <si>
@@ -390,18 +381,12 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">yes -this org type has membership restrictions </t>
-  </si>
-  <si>
     <t>This takes many forms, e.g. a certain percentage of the people who benefit from this orgs activities must be members, or this org only exist through membership</t>
   </si>
   <si>
     <t>donations_deductible</t>
   </si>
   <si>
-    <t>existance_501c</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -492,9 +477,6 @@
     <t>SPECIAL INT GRP</t>
   </si>
   <si>
-    <t>RESTRICTED</t>
-  </si>
-  <si>
     <t>UNLIMITED</t>
   </si>
   <si>
@@ -612,15 +594,6 @@
     <t>organization type can exist as an independent org</t>
   </si>
   <si>
-    <t>just because they are allowed to operate as a intependent org does not restrict an org from voluntarily participating in a group structure - see IRS GEN codes</t>
-  </si>
-  <si>
-    <t>YES - EXEPTIONS</t>
-  </si>
-  <si>
-    <t>org type generally cannot receive donations, but there may be exemptions</t>
-  </si>
-  <si>
     <t>BMF - LEVEL1</t>
   </si>
   <si>
@@ -637,6 +610,60 @@
   </si>
   <si>
     <t>There may be filing requirements that appear on the BMF that are not related to their 501(c) type and thus would not appear in this table.</t>
+  </si>
+  <si>
+    <t>EXCEPTIONS</t>
+  </si>
+  <si>
+    <t>org type generally cannot receive contributions but their may be exceptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org type can receive contribution - unrestricted </t>
+  </si>
+  <si>
+    <t xml:space="preserve">private foundations  are mixed about whether or not they can receive donations. E.g. in the case of a trust.  </t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>yes -this org type has membership restrictions - members are people</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>yes - this org type has membership restrictions - members are other organizations</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>organizations of this type exists as part of a group of organizations to pool resources or assests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">just because they are allowed to operate as a intependent org does not restrict an org from voluntarily participating in a group structure - see IRS GEN codes, </t>
+  </si>
+  <si>
+    <t>A single nonprofit that is a cooperative is not a category "P" organization. Category "P" orgnaization are groups of nonprofits (not people) that pool resources or assests.</t>
   </si>
 </sst>
 </file>
@@ -775,7 +802,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -813,9 +840,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -830,11 +854,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1245,7 +1264,7 @@
     <tableColumn id="7" xr3:uid="{614E85D6-D3FE-4B49-B673-3B96B127C892}" name="donations_deductible" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{C82BB2F4-5690-7E45-9989-0E6197C10A88}" name="political_activity" dataDxfId="8"/>
     <tableColumn id="9" xr3:uid="{77957644-0E53-0447-8131-F726B2193A55}" name="memership_restrictions" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{8EB2C594-11DD-F04E-8BB4-D5AD8A946BA7}" name="existance_501c" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{8EB2C594-11DD-F04E-8BB4-D5AD8A946BA7}" name="supporting" dataDxfId="6"/>
     <tableColumn id="13" xr3:uid="{AD5A5539-ADEA-B747-A32F-06989F8D15A7}" name="other_filing_requirements" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1567,9 +1586,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE3B902-8DA6-D346-AFF8-0B0CB0AD27B0}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="92" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="92" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1592,10 +1611,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="44" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>69</v>
@@ -1604,28 +1623,28 @@
         <v>70</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="M1" s="4"/>
     </row>
@@ -1643,28 +1662,28 @@
         <v>88</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>2</v>
+        <v>201</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>2</v>
+        <v>205</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>199</v>
       </c>
       <c r="M2" s="4"/>
     </row>
@@ -1685,24 +1704,26 @@
         <v>1</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>2</v>
+        <v>195</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" s="11"/>
+        <v>202</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1722,24 +1743,26 @@
         <v>1</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1759,24 +1782,26 @@
         <v>1</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>102</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1796,24 +1821,26 @@
         <v>1</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1833,24 +1860,26 @@
         <v>1</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>102</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1870,24 +1899,26 @@
         <v>1</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>102</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1907,24 +1938,26 @@
         <v>1</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="L9" s="11"/>
+      <c r="L9" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1944,24 +1977,26 @@
         <v>1</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>102</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>1</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1981,24 +2016,26 @@
         <v>1</v>
       </c>
       <c r="F11" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="L11" s="11"/>
+      <c r="L11" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2018,24 +2055,26 @@
         <v>1</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>102</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2055,24 +2094,26 @@
         <v>1</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2092,24 +2133,26 @@
         <v>1</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2126,27 +2169,29 @@
         <v>83</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2166,24 +2211,26 @@
         <v>1</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2203,24 +2250,26 @@
         <v>1</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" s="11"/>
+        <v>204</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2240,24 +2289,26 @@
         <v>1</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>1</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M18" s="4"/>
     </row>
     <row r="19" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2277,24 +2328,26 @@
         <v>1</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L19" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2314,24 +2367,26 @@
         <v>1</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L20" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2360,15 +2415,17 @@
         <v>2</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>2</v>
+        <v>195</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L21" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M21" s="4"/>
     </row>
     <row r="22" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2388,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>1</v>
@@ -2397,15 +2454,17 @@
         <v>102</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>1</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L22" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M22" s="4"/>
     </row>
     <row r="23" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,22 +2484,26 @@
         <v>1</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>102</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="K23" s="13"/>
-      <c r="L23" s="10"/>
+        <v>195</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M23" s="4"/>
     </row>
     <row r="24" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2460,24 +2523,26 @@
         <v>1</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L24" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2506,15 +2571,17 @@
         <v>102</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L25" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M25" s="4"/>
     </row>
     <row r="26" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2534,24 +2601,26 @@
         <v>1</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="L26" s="11"/>
+        <v>202</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M26" s="4"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2568,27 +2637,29 @@
         <v>90</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L27" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M27" s="4"/>
     </row>
     <row r="28" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2605,27 +2676,29 @@
         <v>90</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H28" s="11" t="s">
         <v>102</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L28" s="11"/>
+        <v>205</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M28" s="4"/>
     </row>
     <row r="29" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2645,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>1</v>
@@ -2654,15 +2727,17 @@
         <v>102</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>2</v>
+        <v>110</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L29" s="12"/>
+        <v>205</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M29" s="4"/>
     </row>
     <row r="30" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2682,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>1</v>
@@ -2691,15 +2766,17 @@
         <v>102</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>2</v>
+        <v>110</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L30" s="12"/>
+        <v>205</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M30" s="4"/>
     </row>
     <row r="31" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2727,15 +2804,17 @@
       <c r="H31" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I31" s="16"/>
+      <c r="I31" s="15" t="s">
+        <v>200</v>
+      </c>
       <c r="J31" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>1</v>
+        <v>205</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="M31" s="4"/>
     </row>
@@ -2756,22 +2835,26 @@
         <v>1</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I32" s="16"/>
+        <v>103</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>200</v>
+      </c>
       <c r="J32" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L32" s="6"/>
+        <v>204</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M32" s="4"/>
     </row>
     <row r="33" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2791,22 +2874,26 @@
         <v>1</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I33" s="16"/>
+        <v>103</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>200</v>
+      </c>
       <c r="J33" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L33" s="6"/>
+        <v>204</v>
+      </c>
+      <c r="L33" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M33" s="4"/>
     </row>
     <row r="34" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2826,22 +2913,26 @@
         <v>1</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I34" s="16"/>
+        <v>103</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>200</v>
+      </c>
       <c r="J34" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L34" s="6"/>
+        <v>205</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M34" s="4"/>
     </row>
     <row r="35" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2861,22 +2952,26 @@
         <v>1</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I35" s="16"/>
+        <v>103</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>200</v>
+      </c>
       <c r="J35" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L35" s="6"/>
+        <v>204</v>
+      </c>
+      <c r="L35" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2896,7 +2991,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>1</v>
@@ -2904,14 +2999,18 @@
       <c r="H36" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I36" s="16"/>
-      <c r="J36" s="6" t="s">
-        <v>2</v>
+      <c r="I36" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L36" s="6"/>
+        <v>205</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M36" s="4"/>
     </row>
     <row r="37" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -2939,15 +3038,17 @@
       <c r="H37" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I37" s="16"/>
+      <c r="I37" s="15" t="s">
+        <v>200</v>
+      </c>
       <c r="J37" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>1</v>
+        <v>205</v>
       </c>
       <c r="L37" s="14" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="M37" s="4"/>
     </row>
@@ -2965,21 +3066,29 @@
         <v>96</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
+        <v>132</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>200</v>
+      </c>
       <c r="H38" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I38" s="16"/>
-      <c r="J38" s="6" t="s">
-        <v>2</v>
+      <c r="I38" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L38" s="15"/>
+        <v>205</v>
+      </c>
+      <c r="L38" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="M38" s="4"/>
     </row>
   </sheetData>
@@ -2993,16 +3102,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD4381-EA25-4248-8CB2-EADFAADE5A2B}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="22" customWidth="1"/>
-    <col min="2" max="3" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="85" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="67.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
@@ -3010,250 +3120,253 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>160</v>
+        <v>168</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>154</v>
       </c>
       <c r="D1" t="s">
         <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
-        <v>161</v>
+      <c r="A2" s="21" t="s">
+        <v>155</v>
       </c>
       <c r="B2" t="s">
         <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D2" t="s">
         <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>194</v>
+        <v>163</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>161</v>
+      <c r="A3" s="21" t="s">
+        <v>155</v>
       </c>
       <c r="B3" t="s">
         <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>194</v>
+      <c r="E3" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>162</v>
+      <c r="A4" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="B4" t="s">
         <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>194</v>
+      <c r="E4" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>162</v>
+      <c r="A5" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="B5" t="s">
         <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>169</v>
+      <c r="E5" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>162</v>
+      <c r="A6" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="B6" t="s">
         <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D6" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>169</v>
+      <c r="E6" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
-        <v>162</v>
+      <c r="A7" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="B7" t="s">
         <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D7" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>169</v>
+      <c r="E7" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>162</v>
+      <c r="A8" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="B8" t="s">
         <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>169</v>
+      <c r="E8" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>162</v>
+      <c r="A9" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="B9" t="s">
         <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D9" t="s">
         <v>97</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>169</v>
+      <c r="E9" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
-        <v>162</v>
+      <c r="A10" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="B10" t="s">
         <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D10" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>169</v>
+      <c r="E10" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
-        <v>162</v>
+      <c r="A11" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="B11" t="s">
         <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D11" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>169</v>
+      <c r="E11" s="22" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
-        <v>167</v>
+      <c r="A12" s="20" t="s">
+        <v>161</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>193</v>
       </c>
       <c r="E12" t="s">
-        <v>170</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>195</v>
+        <v>164</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
-        <v>167</v>
+      <c r="A13" s="20" t="s">
+        <v>161</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>191</v>
       </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>192</v>
       </c>
       <c r="E13" t="s">
-        <v>170</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>195</v>
+        <v>164</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="G13" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
-        <v>167</v>
+      <c r="A14" s="20" t="s">
+        <v>161</v>
       </c>
       <c r="B14" t="s">
         <v>102</v>
@@ -3262,129 +3375,123 @@
         <v>102</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E14" t="s">
-        <v>170</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>195</v>
+        <v>164</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>186</v>
       </c>
       <c r="G14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
-        <v>167</v>
+      <c r="A15" s="20" t="s">
+        <v>161</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E15" t="s">
-        <v>170</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>195</v>
+        <v>164</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>186</v>
       </c>
       <c r="G15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="C16" t="s">
-        <v>192</v>
+        <v>108</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="D16" t="s">
-        <v>193</v>
-      </c>
-      <c r="E16" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F16" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="G16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" t="s">
+        <v>197</v>
+      </c>
+      <c r="G19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="D17" t="s">
-        <v>186</v>
-      </c>
-      <c r="F17" s="18" t="s">
+      <c r="C20" t="s">
         <v>196</v>
       </c>
-      <c r="G17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="D18" t="s">
-        <v>187</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" t="s">
-        <v>116</v>
-      </c>
       <c r="D20" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20" t="s">
-        <v>118</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
-        <v>163</v>
+      <c r="A21" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -3393,309 +3500,323 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E21" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
-        <v>163</v>
+      <c r="A22" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D23" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" t="s">
+        <v>164</v>
+      </c>
+      <c r="G23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" t="s">
+        <v>204</v>
+      </c>
+      <c r="D26" t="s">
+        <v>206</v>
+      </c>
+      <c r="G26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+      <c r="E27" t="s">
         <v>164</v>
       </c>
-      <c r="B23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="F27" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" t="s">
+        <v>169</v>
+      </c>
+      <c r="D28" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" t="s">
+        <v>164</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" t="s">
+        <v>164</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E31" t="s">
+        <v>164</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G31" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" t="s">
+        <v>164</v>
+      </c>
+      <c r="F36" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="E23" t="s">
-        <v>170</v>
-      </c>
-      <c r="G23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E37" t="s">
         <v>164</v>
       </c>
-      <c r="B24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" t="s">
-        <v>155</v>
-      </c>
-      <c r="D24" t="s">
-        <v>122</v>
-      </c>
-      <c r="E24" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
+      <c r="F37" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" t="s">
+        <v>179</v>
+      </c>
+      <c r="E38" t="s">
         <v>164</v>
       </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" t="s">
-        <v>190</v>
-      </c>
-      <c r="E25" t="s">
-        <v>170</v>
-      </c>
-      <c r="G25" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="B26" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" t="s">
-        <v>173</v>
-      </c>
-      <c r="D26" t="s">
-        <v>176</v>
-      </c>
-      <c r="E26" t="s">
-        <v>170</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C27" t="s">
-        <v>175</v>
-      </c>
-      <c r="D27" t="s">
-        <v>177</v>
-      </c>
-      <c r="E27" t="s">
-        <v>170</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" t="s">
-        <v>125</v>
-      </c>
-      <c r="E28" t="s">
-        <v>170</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" t="s">
-        <v>170</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="D30" t="s">
-        <v>181</v>
-      </c>
-      <c r="E30" t="s">
-        <v>170</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="G30" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B31" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B33" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" t="s">
-        <v>170</v>
-      </c>
-      <c r="G33" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="D34" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" t="s">
-        <v>170</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="B35" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35" t="s">
-        <v>157</v>
-      </c>
-      <c r="D35" t="s">
-        <v>183</v>
-      </c>
-      <c r="E35" t="s">
-        <v>170</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="B36" t="s">
-        <v>137</v>
-      </c>
-      <c r="C36" t="s">
-        <v>158</v>
-      </c>
-      <c r="D36" t="s">
-        <v>184</v>
-      </c>
-      <c r="E36" t="s">
-        <v>170</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>159</v>
-      </c>
-      <c r="D37" t="s">
-        <v>185</v>
-      </c>
-      <c r="E37" t="s">
-        <v>170</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>198</v>
+      <c r="F38" s="16" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
looking more into donations_deductible
</commit_message>
<xml_diff>
--- a/tax-exempt-status/501ctypes.xlsx
+++ b/tax-exempt-status/501ctypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviabeck/Box Sync/metadata-standards/tax-exempt-status/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870AF53C-D0E9-5341-845E-7D195EF611B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56692F42-495C-D342-A214-81CC5F4946FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{96359B12-0556-B241-B8CB-31DA73770B59}"/>
   </bookViews>
@@ -621,9 +621,6 @@
     <t xml:space="preserve">org type can receive contribution - unrestricted </t>
   </si>
   <si>
-    <t xml:space="preserve">private foundations  are mixed about whether or not they can receive donations. E.g. in the case of a trust.  </t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
@@ -664,6 +661,9 @@
   </si>
   <si>
     <t>A single nonprofit that is a cooperative is not a category "P" organization. Category "P" orgnaization are groups of nonprofits (not people) that pool resources or assests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">private foundations  are mixed about whether or not they can receive donations. E.g. in the case of a trust.  Cemetaries, </t>
   </si>
 </sst>
 </file>
@@ -802,7 +802,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -853,6 +853,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1586,9 +1589,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE3B902-8DA6-D346-AFF8-0B0CB0AD27B0}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="92" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
       <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B31" sqref="B31"/>
+      <selection pane="topRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1668,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>166</v>
@@ -1677,13 +1680,13 @@
         <v>110</v>
       </c>
       <c r="J2" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="M2" s="4"/>
     </row>
@@ -1716,13 +1719,13 @@
         <v>109</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M3" s="4"/>
     </row>
@@ -1758,10 +1761,10 @@
         <v>1</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M4" s="4"/>
     </row>
@@ -1797,10 +1800,10 @@
         <v>1</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M5" s="4"/>
     </row>
@@ -1836,10 +1839,10 @@
         <v>113</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M6" s="4"/>
     </row>
@@ -1875,10 +1878,10 @@
         <v>1</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M7" s="4"/>
     </row>
@@ -1914,10 +1917,10 @@
         <v>1</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M8" s="4"/>
     </row>
@@ -1943,7 +1946,7 @@
       <c r="G9" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="13" t="s">
         <v>166</v>
       </c>
       <c r="I9" s="10" t="s">
@@ -1956,7 +1959,7 @@
         <v>116</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M9" s="4"/>
     </row>
@@ -1992,10 +1995,10 @@
         <v>1</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M10" s="4"/>
     </row>
@@ -2021,7 +2024,7 @@
       <c r="G11" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="13" t="s">
         <v>166</v>
       </c>
       <c r="I11" s="10" t="s">
@@ -2034,7 +2037,7 @@
         <v>116</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M11" s="4"/>
     </row>
@@ -2070,10 +2073,10 @@
         <v>113</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M12" s="4"/>
     </row>
@@ -2109,10 +2112,10 @@
         <v>113</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M13" s="4"/>
     </row>
@@ -2138,8 +2141,8 @@
       <c r="G14" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>103</v>
+      <c r="H14" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>110</v>
@@ -2148,10 +2151,10 @@
         <v>113</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M14" s="4"/>
     </row>
@@ -2187,10 +2190,10 @@
         <v>113</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M15" s="4"/>
     </row>
@@ -2226,10 +2229,10 @@
         <v>113</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M16" s="4"/>
     </row>
@@ -2265,10 +2268,10 @@
         <v>113</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M17" s="4"/>
     </row>
@@ -2304,10 +2307,10 @@
         <v>1</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M18" s="4"/>
     </row>
@@ -2343,10 +2346,10 @@
         <v>113</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M19" s="4"/>
     </row>
@@ -2372,7 +2375,7 @@
       <c r="G20" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="23" t="s">
         <v>103</v>
       </c>
       <c r="I20" s="10" t="s">
@@ -2382,10 +2385,10 @@
         <v>113</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M20" s="4"/>
     </row>
@@ -2418,13 +2421,13 @@
         <v>110</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M21" s="4"/>
     </row>
@@ -2460,10 +2463,10 @@
         <v>1</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M22" s="4"/>
     </row>
@@ -2496,13 +2499,13 @@
         <v>110</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M23" s="4"/>
     </row>
@@ -2538,10 +2541,10 @@
         <v>113</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M24" s="4"/>
     </row>
@@ -2574,13 +2577,13 @@
         <v>110</v>
       </c>
       <c r="J25" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="L25" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="L25" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="M25" s="4"/>
     </row>
@@ -2613,13 +2616,13 @@
         <v>110</v>
       </c>
       <c r="J26" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="L26" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="M26" s="4"/>
     </row>
@@ -2652,13 +2655,13 @@
         <v>110</v>
       </c>
       <c r="J27" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="L27" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="L27" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="M27" s="4"/>
     </row>
@@ -2694,10 +2697,10 @@
         <v>113</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M28" s="4"/>
     </row>
@@ -2730,13 +2733,13 @@
         <v>110</v>
       </c>
       <c r="J29" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="L29" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="L29" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="M29" s="4"/>
     </row>
@@ -2769,13 +2772,13 @@
         <v>110</v>
       </c>
       <c r="J30" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="L30" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="L30" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="M30" s="4"/>
     </row>
@@ -2805,13 +2808,13 @@
         <v>102</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>113</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>128</v>
@@ -2844,16 +2847,16 @@
         <v>103</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L32" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M32" s="4"/>
     </row>
@@ -2883,16 +2886,16 @@
         <v>103</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>113</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L33" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M33" s="4"/>
     </row>
@@ -2922,16 +2925,16 @@
         <v>103</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>1</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L34" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M34" s="4"/>
     </row>
@@ -2961,16 +2964,16 @@
         <v>103</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>113</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L35" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M35" s="4"/>
     </row>
@@ -3000,16 +3003,16 @@
         <v>102</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J36" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="L36" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="L36" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="M36" s="4"/>
     </row>
@@ -3039,13 +3042,13 @@
         <v>102</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>113</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L37" s="14" t="s">
         <v>129</v>
@@ -3069,25 +3072,25 @@
         <v>132</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>102</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J38" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="L38" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="K38" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="L38" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="M38" s="4"/>
     </row>
@@ -3104,8 +3107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD4381-EA25-4248-8CB2-EADFAADE5A2B}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="G3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3361,7 +3364,7 @@
         <v>186</v>
       </c>
       <c r="G13" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -3469,7 +3472,7 @@
         <v>113</v>
       </c>
       <c r="D19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G19" t="s">
         <v>114</v>
@@ -3480,13 +3483,13 @@
         <v>157</v>
       </c>
       <c r="B20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" t="s">
         <v>195</v>
       </c>
-      <c r="C20" t="s">
-        <v>196</v>
-      </c>
       <c r="D20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3525,7 +3528,7 @@
         <v>158</v>
       </c>
       <c r="B23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>159</v>
@@ -3562,7 +3565,7 @@
         <v>158</v>
       </c>
       <c r="B25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C25" t="s">
         <v>150</v>
@@ -3574,7 +3577,7 @@
         <v>164</v>
       </c>
       <c r="G25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -3582,13 +3585,13 @@
         <v>158</v>
       </c>
       <c r="B26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>